<commit_message>
Uploading results for assignment 3 and organizing git master root
- Created and uploaded first version of assignment 3 files (deliverable
docx and excel file)
- Reorganized Assignment 1 inside a folder.
- Moved assignment 2 documents to Assignment 2 folder.
</commit_message>
<xml_diff>
--- a/Assignment2/Assignment2Team2.xlsx
+++ b/Assignment2/Assignment2Team2.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="Results" sheetId="5" r:id="rId1"/>
-    <sheet name="Lucene (Title_Description_Both)" sheetId="2" r:id="rId2"/>
-    <sheet name="Eclipse (Both)" sheetId="1" r:id="rId3"/>
-    <sheet name="Eclipse (Description)" sheetId="4" r:id="rId4"/>
-    <sheet name="Eclipse (Title)" sheetId="3" r:id="rId5"/>
+    <sheet name="Apache Lucene Results" sheetId="5" r:id="rId1"/>
+    <sheet name="Eclipse JDT Core Results" sheetId="6" r:id="rId2"/>
+    <sheet name="Lucene (Title_Description_Both)" sheetId="2" r:id="rId3"/>
+    <sheet name="Eclipse (Both)" sheetId="1" r:id="rId4"/>
+    <sheet name="Eclipse (Description)" sheetId="4" r:id="rId5"/>
+    <sheet name="Eclipse (Title)" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1653" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1727" uniqueCount="620">
   <si>
     <t>TITLE : ************************************</t>
   </si>
@@ -1842,9 +1843,6 @@
     <t>Eclipse JDT Core 4.5</t>
   </si>
   <si>
-    <t>Lucene 5.4</t>
-  </si>
-  <si>
     <t>Bug 1 - Title Only</t>
   </si>
   <si>
@@ -1873,6 +1871,24 @@
   </si>
   <si>
     <t>Bug 5 - Desc Only</t>
+  </si>
+  <si>
+    <t>Across Systems</t>
+  </si>
+  <si>
+    <t>Apache Lucene 5.4</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>1/0</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>18</t>
   </si>
 </sst>
 </file>
@@ -2146,7 +2162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2192,26 +2208,8 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2247,6 +2245,42 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2537,17 +2571,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="7" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="10.140625" bestFit="1" customWidth="1"/>
@@ -2555,27 +2590,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="36" t="s">
         <v>578</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>603</v>
-      </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="23" t="s">
-        <v>604</v>
-      </c>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="25"/>
+      <c r="B1" s="38" t="s">
+        <v>615</v>
+      </c>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="38" t="s">
+        <v>614</v>
+      </c>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="41"/>
       <c r="P1" s="7"/>
       <c r="Q1" s="7"/>
       <c r="R1" s="7"/>
@@ -2583,47 +2618,47 @@
       <c r="T1" s="7"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
+      <c r="A2" s="37"/>
       <c r="B2" s="16" t="s">
         <v>579</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="21" t="s">
         <v>580</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="21" t="s">
         <v>581</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="21" t="s">
         <v>582</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="21" t="s">
         <v>583</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="21" t="s">
         <v>584</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="22" t="s">
         <v>559</v>
       </c>
       <c r="I2" s="16" t="s">
         <v>579</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="21" t="s">
         <v>580</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="21" t="s">
         <v>581</v>
       </c>
-      <c r="L2" s="26" t="s">
+      <c r="L2" s="21" t="s">
         <v>582</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="M2" s="21" t="s">
         <v>583</v>
       </c>
-      <c r="N2" s="26" t="s">
+      <c r="N2" s="21" t="s">
         <v>584</v>
       </c>
-      <c r="O2" s="27" t="s">
+      <c r="O2" s="22" t="s">
         <v>559</v>
       </c>
       <c r="P2" s="7"/>
@@ -2634,16 +2669,16 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>605</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>604</v>
+      </c>
+      <c r="B3" s="28"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="34"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="28"/>
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
@@ -2658,16 +2693,16 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>606</v>
-      </c>
-      <c r="B4" s="8"/>
+        <v>605</v>
+      </c>
+      <c r="B4" s="29"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="35"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="29"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
@@ -2682,16 +2717,16 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>607</v>
-      </c>
-      <c r="B5" s="8"/>
+        <v>606</v>
+      </c>
+      <c r="B5" s="29"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="35"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="29"/>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
@@ -2706,16 +2741,30 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>608</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="36" t="s">
+        <v>607</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>590</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>591</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>597</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>597</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>597</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>598</v>
+      </c>
+      <c r="I6" s="30" t="s">
         <v>590</v>
       </c>
       <c r="J6" s="9" t="s">
@@ -2744,16 +2793,16 @@
     </row>
     <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>609</v>
-      </c>
-      <c r="B7" s="17"/>
+        <v>608</v>
+      </c>
+      <c r="B7" s="31"/>
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="37"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="31"/>
       <c r="J7" s="17"/>
       <c r="K7" s="17"/>
       <c r="L7" s="17"/>
@@ -2768,20 +2817,34 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>610</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="36" t="s">
+        <v>609</v>
+      </c>
+      <c r="B8" s="30" t="s">
         <v>595</v>
       </c>
+      <c r="C8" s="9" t="s">
+        <v>595</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>595</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>595</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>596</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>595</v>
+      </c>
       <c r="J8" s="9" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="K8" s="9" t="s">
         <v>592</v>
@@ -2790,13 +2853,13 @@
         <v>595</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>595</v>
+        <v>617</v>
       </c>
       <c r="N8" s="9" t="s">
         <v>593</v>
       </c>
       <c r="O8" s="15" t="s">
-        <v>596</v>
+        <v>618</v>
       </c>
       <c r="P8" s="7"/>
       <c r="Q8" s="7"/>
@@ -2806,50 +2869,36 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>611</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>590</v>
-      </c>
-      <c r="C9" s="9" t="s">
+        <v>610</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>595</v>
+      </c>
+      <c r="C9" s="34" t="s">
         <v>591</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="34" t="s">
         <v>592</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>593</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>593</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>593</v>
-      </c>
-      <c r="H9" s="33" t="s">
-        <v>594</v>
-      </c>
-      <c r="I9" s="39" t="s">
+      <c r="E9" s="34" t="s">
         <v>595</v>
       </c>
-      <c r="J9" s="40" t="s">
-        <v>591</v>
-      </c>
-      <c r="K9" s="40" t="s">
-        <v>592</v>
-      </c>
-      <c r="L9" s="40" t="s">
-        <v>595</v>
-      </c>
-      <c r="M9" s="40" t="s">
+      <c r="F9" s="34" t="s">
         <v>599</v>
       </c>
-      <c r="N9" s="40" t="s">
+      <c r="G9" s="34" t="s">
         <v>599</v>
       </c>
-      <c r="O9" s="41" t="s">
+      <c r="H9" s="35" t="s">
         <v>600</v>
       </c>
+      <c r="I9" s="45"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="46"/>
+      <c r="O9" s="47"/>
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
@@ -2858,36 +2907,36 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>612</v>
-      </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="36" t="s">
+        <v>611</v>
+      </c>
+      <c r="B10" s="30" t="s">
         <v>595</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="C10" s="9" t="s">
         <v>595</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>592</v>
       </c>
-      <c r="L10" s="9" t="s">
+      <c r="E10" s="9" t="s">
         <v>595</v>
       </c>
-      <c r="M10" s="9" t="s">
+      <c r="F10" s="9" t="s">
         <v>595</v>
       </c>
-      <c r="N10" s="9" t="s">
+      <c r="G10" s="9" t="s">
         <v>597</v>
       </c>
-      <c r="O10" s="15" t="s">
+      <c r="H10" s="15" t="s">
         <v>601</v>
       </c>
+      <c r="I10" s="29"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="14"/>
       <c r="P10" s="7"/>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
@@ -2896,16 +2945,16 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>613</v>
-      </c>
-      <c r="B11" s="8"/>
+        <v>612</v>
+      </c>
+      <c r="B11" s="29"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="35"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="29"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
@@ -2920,16 +2969,30 @@
     </row>
     <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
-        <v>614</v>
-      </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="38" t="s">
+        <v>613</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>595</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>595</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>592</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>595</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>595</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>599</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>601</v>
+      </c>
+      <c r="I12" s="32" t="s">
         <v>595</v>
       </c>
       <c r="J12" s="19" t="s">
@@ -2948,7 +3011,7 @@
         <v>599</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>601</v>
+        <v>619</v>
       </c>
       <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
@@ -2960,14 +3023,14 @@
       <c r="A13" s="10" t="s">
         <v>585</v>
       </c>
-      <c r="B13" s="11"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="34"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="28"/>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
@@ -2984,11 +3047,11 @@
       <c r="A14" s="13" t="s">
         <v>586</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="30" t="s">
         <v>595</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>592</v>
@@ -2997,35 +3060,21 @@
         <v>595</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>595</v>
+        <v>599</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>593</v>
-      </c>
-      <c r="H14" s="33" t="s">
-        <v>596</v>
-      </c>
-      <c r="I14" s="36" t="s">
-        <v>595</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>591</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>592</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>595</v>
-      </c>
-      <c r="M14" s="9" t="s">
         <v>599</v>
       </c>
-      <c r="N14" s="9" t="s">
-        <v>599</v>
-      </c>
-      <c r="O14" s="15" t="s">
+      <c r="H14" s="15" t="s">
         <v>600</v>
       </c>
+      <c r="I14" s="29"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="14"/>
       <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
       <c r="R14" s="7"/>
@@ -3036,34 +3085,34 @@
       <c r="A15" s="13" t="s">
         <v>587</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="36" t="s">
+      <c r="B15" s="30" t="s">
         <v>595</v>
       </c>
-      <c r="J15" s="9" t="s">
+      <c r="C15" s="9" t="s">
         <v>595</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="D15" s="9" t="s">
         <v>602</v>
       </c>
-      <c r="L15" s="9" t="s">
+      <c r="E15" s="9" t="s">
         <v>595</v>
       </c>
-      <c r="M15" s="9" t="s">
+      <c r="F15" s="9" t="s">
         <v>595</v>
       </c>
-      <c r="N15" s="9" t="s">
+      <c r="G15" s="9" t="s">
         <v>597</v>
       </c>
-      <c r="O15" s="15" t="s">
+      <c r="H15" s="15" t="s">
         <v>601</v>
       </c>
+      <c r="I15" s="29"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="14"/>
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
@@ -3074,15 +3123,29 @@
       <c r="A16" s="13" t="s">
         <v>588</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="36" t="s">
+      <c r="B16" s="30" t="s">
         <v>590</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>591</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>597</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>597</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>597</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>594</v>
+      </c>
+      <c r="I16" s="30" t="s">
+        <v>595</v>
       </c>
       <c r="J16" s="9" t="s">
         <v>591</v>
@@ -3091,7 +3154,7 @@
         <v>592</v>
       </c>
       <c r="L16" s="9" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="M16" s="9" t="s">
         <v>597</v>
@@ -3100,7 +3163,7 @@
         <v>597</v>
       </c>
       <c r="O16" s="15" t="s">
-        <v>594</v>
+        <v>600</v>
       </c>
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
@@ -3112,14 +3175,14 @@
       <c r="A17" s="16" t="s">
         <v>589</v>
       </c>
-      <c r="B17" s="17"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="37"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="31"/>
       <c r="J17" s="17"/>
       <c r="K17" s="17"/>
       <c r="L17" s="17"/>
@@ -3298,6 +3361,685 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="7" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>578</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>603</v>
+      </c>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="38" t="s">
+        <v>614</v>
+      </c>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+    </row>
+    <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="37"/>
+      <c r="B2" s="16" t="s">
+        <v>579</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>580</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>581</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>582</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>583</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>584</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>559</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>579</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>580</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>581</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>582</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>583</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>584</v>
+      </c>
+      <c r="O2" s="22" t="s">
+        <v>559</v>
+      </c>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>604</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>605</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>606</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>607</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+    </row>
+    <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
+        <v>608</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>609</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>610</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>590</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>591</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>594</v>
+      </c>
+      <c r="I9" s="42" t="s">
+        <v>595</v>
+      </c>
+      <c r="J9" s="43" t="s">
+        <v>591</v>
+      </c>
+      <c r="K9" s="43" t="s">
+        <v>592</v>
+      </c>
+      <c r="L9" s="43" t="s">
+        <v>595</v>
+      </c>
+      <c r="M9" s="43" t="s">
+        <v>593</v>
+      </c>
+      <c r="N9" s="43" t="s">
+        <v>593</v>
+      </c>
+      <c r="O9" s="44" t="s">
+        <v>600</v>
+      </c>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>611</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>612</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+    </row>
+    <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
+        <v>613</v>
+      </c>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>585</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>586</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>595</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>595</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>595</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>595</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="H14" s="27" t="s">
+        <v>596</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>595</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>595</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>595</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>595</v>
+      </c>
+      <c r="N14" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="O14" s="44" t="s">
+        <v>616</v>
+      </c>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>587</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>588</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+    </row>
+    <row r="17" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
+        <v>589</v>
+      </c>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="I1:O1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B492"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6521,7 +7263,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C204"/>
   <sheetViews>
@@ -7789,11 +8531,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C202"/>
   <sheetViews>
-    <sheetView topLeftCell="A196" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A59" sqref="A59:B61"/>
     </sheetView>
   </sheetViews>
@@ -8999,12 +9741,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B138"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A138" sqref="A138"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>